<commit_message>
Updated Project 3 with Rubric and other visuals
</commit_message>
<xml_diff>
--- a/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Screenshots as per Rubric/Rubric tracker.xlsx
+++ b/Udacity Preparing and Modelling Data/Project 3 Project Market Analysis Report for National Clothing Chain/Screenshots as per Rubric/Rubric tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PowerBI\Power-BI\Udacity Preparing and Modelling Data\Project 3 Project Market Analysis Report for National Clothing Chain\Screenshots as per Rubric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD01F1E4-CC47-44AD-9CB0-FA4D1B0B4506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB94D2EA-E627-4EF6-A729-2E5D264E15E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20617" yWindow="-3405" windowWidth="20715" windowHeight="13875" xr2:uid="{0E040457-2FD3-47A4-81B4-7EB53601751D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>CRITERIA</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>3 Predicted Customer Income Bins DAX formula</t>
+  </si>
+  <si>
+    <t>4 Targeted Customer Income Bins DAX formula</t>
+  </si>
+  <si>
+    <t>5 Predicted customer Income linear regression formula</t>
+  </si>
+  <si>
+    <t>6 Histogram of Predicted customer Income</t>
+  </si>
+  <si>
+    <t>7 Scatter plot with trendline and correlation coefficient card - Sales and Income</t>
   </si>
 </sst>
 </file>
@@ -357,10 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -379,6 +388,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD328A0-A231-4F37-9A45-D654683D7BC9}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,10 +719,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -718,444 +730,456 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="C20" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="C23" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
+      <c r="C26" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B54" s="6" t="s">
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B54" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B59" s="6"/>
+      <c r="B59" s="5"/>
     </row>
     <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B67" s="6"/>
+      <c r="B67" s="5"/>
     </row>
     <row r="68" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="75" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="5" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>